<commit_message>
move header footer spreadsheets
</commit_message>
<xml_diff>
--- a/1866-1873-Field-Diaries/LJs/previous/Last Journals Headers and Footers Vol 1.xlsx
+++ b/1866-1873-Field-Diaries/LJs/previous/Last Journals Headers and Footers Vol 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24520" windowHeight="15380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Headers" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="280">
   <si>
     <t>xvk</t>
   </si>
@@ -670,9 +670,6 @@
     <t>P2</t>
   </si>
   <si>
-    <t>Note: I'm assuming this is the case, as the scan of this page is messed up.</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -722,6 +719,147 @@
   </si>
   <si>
     <t>2A2</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;a2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;B&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;B2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;C&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;C2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;D&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;D2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;E&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;E2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;F&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;F2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;G&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;G2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;H&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;H2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;I&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;I2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;K&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;K2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;L&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;L2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;M&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;M2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;N&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;N2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;O&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;O2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;P&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;P2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;Q&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;Q1&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;R&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;R2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;S&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;S2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;T&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;T2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;U&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;U2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;X&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;X2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;Y&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;Y2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;Z&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;Z2&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw type="catch"&gt;&lt;seg rend="smallcaps"&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend="right"&gt;2A&lt;/seg&gt;&lt;/fw&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fw place="inspace"&gt;&lt;seg rend="right"&gt;2A2&lt;/seg&gt;&lt;/fw&gt;</t>
   </si>
 </sst>
 </file>
@@ -777,8 +915,210 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="305">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -895,7 +1235,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="305">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -947,6 +1287,107 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -998,6 +1439,107 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5270,463 +5812,793 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="D1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>9</v>
+      </c>
       <c r="C2" t="s">
         <v>184</v>
       </c>
-      <c r="D2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="D2" t="str">
+        <f>"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C2&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;a2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
         <v>186</v>
       </c>
       <c r="C3" t="s">
         <v>185</v>
       </c>
-      <c r="D3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" t="str">
+        <f>"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C3&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;B&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>29</v>
+      </c>
       <c r="C4" t="s">
         <v>187</v>
       </c>
-      <c r="D4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="D4" t="str">
+        <f t="shared" ref="D4" si="0">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C4&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;B2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
         <v>186</v>
       </c>
       <c r="C5" t="s">
         <v>189</v>
       </c>
-      <c r="D5">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" t="str">
+        <f t="shared" ref="D5" si="1">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C5&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;C&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>41</v>
+      </c>
       <c r="C6" t="s">
         <v>191</v>
       </c>
-      <c r="D6">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="D6" t="str">
+        <f t="shared" ref="D6" si="2">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C6&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;C2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
         <v>186</v>
       </c>
       <c r="C7" t="s">
         <v>190</v>
       </c>
-      <c r="D7">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" t="str">
+        <f t="shared" ref="D7" si="3">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C7&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;D&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>57</v>
+      </c>
       <c r="C8" t="s">
         <v>192</v>
       </c>
-      <c r="D8">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
+      <c r="D8" t="str">
+        <f t="shared" ref="D8" si="4">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C8&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;D2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>71</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C9" t="s">
         <v>193</v>
       </c>
-      <c r="D9">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" t="str">
+        <f t="shared" ref="D9" si="5">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C9&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;E&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>73</v>
+      </c>
       <c r="C10" t="s">
         <v>194</v>
       </c>
-      <c r="D10">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
+      <c r="D10" t="str">
+        <f t="shared" ref="D10" si="6">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C10&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;E2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>91</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C11" t="s">
         <v>195</v>
       </c>
-      <c r="D11">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" t="str">
+        <f t="shared" ref="D11" si="7">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C11&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;F&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>93</v>
+      </c>
       <c r="C12" t="s">
         <v>196</v>
       </c>
-      <c r="D12">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
+      <c r="D12" t="str">
+        <f t="shared" ref="D12" si="8">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C12&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;F2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>107</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C13" t="s">
         <v>197</v>
       </c>
-      <c r="D13">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D13" t="str">
+        <f t="shared" ref="D13" si="9">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C13&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;G&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>109</v>
+      </c>
       <c r="C14" t="s">
         <v>198</v>
       </c>
-      <c r="D14">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
+      <c r="D14" t="str">
+        <f t="shared" ref="D14" si="10">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C14&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;G2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E14" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>123</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C15" t="s">
         <v>199</v>
       </c>
-      <c r="D15">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="D15" t="str">
+        <f t="shared" ref="D15" si="11">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C15&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;H&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>125</v>
+      </c>
       <c r="C16" t="s">
         <v>200</v>
       </c>
-      <c r="D16">
-        <v>125</v>
+      <c r="D16" t="str">
+        <f t="shared" ref="D16" si="12">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C16&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;H2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E16" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="1" t="s">
+      <c r="A17">
+        <v>139</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C17" t="s">
         <v>201</v>
       </c>
-      <c r="D17">
-        <v>139</v>
+      <c r="D17" t="str">
+        <f t="shared" ref="D17" si="13">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C17&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;I&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E17" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:5">
+      <c r="A18">
+        <v>141</v>
+      </c>
       <c r="C18" t="s">
         <v>202</v>
       </c>
-      <c r="D18">
-        <v>141</v>
+      <c r="D18" t="str">
+        <f t="shared" ref="D18" si="14">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C18&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;I2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E18" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
+      <c r="A19">
+        <v>155</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C19" t="s">
         <v>203</v>
       </c>
-      <c r="D19">
-        <v>155</v>
+      <c r="D19" t="str">
+        <f t="shared" ref="D19" si="15">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C19&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;K&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E19" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:5">
+      <c r="A20">
+        <v>157</v>
+      </c>
       <c r="C20" t="s">
         <v>204</v>
       </c>
-      <c r="D20">
-        <v>157</v>
+      <c r="D20" t="str">
+        <f t="shared" ref="D20" si="16">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C20&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;K2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E20" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
+      <c r="A21">
+        <v>171</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C21" t="s">
         <v>205</v>
       </c>
-      <c r="D21">
-        <v>171</v>
+      <c r="D21" t="str">
+        <f t="shared" ref="D21" si="17">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C21&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;L&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E21" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:5">
+      <c r="A22">
+        <v>173</v>
+      </c>
       <c r="C22" t="s">
         <v>206</v>
       </c>
-      <c r="D22">
-        <v>173</v>
+      <c r="D22" t="str">
+        <f t="shared" ref="D22" si="18">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C22&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;L2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E22" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" t="s">
+      <c r="A23">
+        <v>187</v>
+      </c>
+      <c r="B23" t="s">
         <v>186</v>
       </c>
       <c r="C23" t="s">
         <v>207</v>
       </c>
-      <c r="D23">
-        <v>187</v>
+      <c r="D23" t="str">
+        <f t="shared" ref="D23" si="19">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C23&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;M&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E23" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="24" spans="1:5">
+      <c r="A24">
+        <v>189</v>
+      </c>
       <c r="C24" t="s">
         <v>208</v>
       </c>
-      <c r="D24">
-        <v>189</v>
+      <c r="D24" t="str">
+        <f t="shared" ref="D24" si="20">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C24&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;M2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E24" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="1" t="s">
+      <c r="A25">
+        <v>203</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C25" t="s">
         <v>209</v>
       </c>
-      <c r="D25">
-        <v>203</v>
+      <c r="D25" t="str">
+        <f t="shared" ref="D25" si="21">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C25&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;N&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E25" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="26" spans="1:5">
+      <c r="A26">
+        <v>205</v>
+      </c>
       <c r="C26" t="s">
         <v>210</v>
       </c>
-      <c r="D26">
-        <v>205</v>
+      <c r="D26" t="str">
+        <f t="shared" ref="D26" si="22">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C26&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;N2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E26" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="1" t="s">
+      <c r="A27">
+        <v>221</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C27" t="s">
         <v>211</v>
       </c>
-      <c r="D27">
-        <v>221</v>
+      <c r="D27" t="str">
+        <f t="shared" ref="D27" si="23">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C27&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;O&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E27" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="28" spans="1:5">
+      <c r="A28">
+        <v>223</v>
+      </c>
       <c r="C28" t="s">
         <v>212</v>
       </c>
-      <c r="D28">
-        <v>223</v>
+      <c r="D28" t="str">
+        <f t="shared" ref="D28" si="24">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C28&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;O2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E28" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="1" t="s">
+      <c r="A29">
+        <v>239</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C29" t="s">
         <v>214</v>
       </c>
-      <c r="D29">
-        <v>239</v>
+      <c r="D29" t="str">
+        <f t="shared" ref="D29" si="25">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C29&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;P&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E29" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:5">
+      <c r="A30">
+        <v>241</v>
+      </c>
       <c r="C30" t="s">
         <v>215</v>
       </c>
-      <c r="D30">
-        <v>241</v>
+      <c r="D30" t="str">
+        <f t="shared" ref="D30" si="26">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C30&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;P2&lt;/seg&gt;&lt;/fw&gt;</v>
       </c>
       <c r="E30" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="1" t="s">
+      <c r="A31">
+        <v>255</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C31" t="s">
         <v>213</v>
       </c>
-      <c r="D31">
-        <v>255</v>
+      <c r="D31" t="str">
+        <f t="shared" ref="D31" si="27">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C31&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;Q&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E31" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:5">
+      <c r="A32">
+        <v>257</v>
+      </c>
       <c r="C32" t="s">
+        <v>216</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" ref="D32" si="28">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C32&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;Q1&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E32" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>273</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" t="s">
         <v>217</v>
       </c>
-      <c r="D32">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
+      <c r="D33" t="str">
+        <f t="shared" ref="D33" si="29">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C33&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;R&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E33" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>275</v>
+      </c>
+      <c r="C34" t="s">
+        <v>218</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" ref="D34" si="30">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C34&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;R2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E34" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>289</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C33" t="s">
-        <v>218</v>
-      </c>
-      <c r="D33">
+      <c r="C35" t="s">
+        <v>219</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" ref="D35" si="31">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C35&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;S&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E35" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>291</v>
+      </c>
+      <c r="C36" t="s">
+        <v>220</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" ref="D36" si="32">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C36&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;S2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E36" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>305</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C37" t="s">
+        <v>221</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" ref="D37" si="33">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C37&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;T&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E37" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>307</v>
+      </c>
+      <c r="C38" t="s">
+        <v>222</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" ref="D38" si="34">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C38&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;T2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E38" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>321</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" t="s">
+        <v>223</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" ref="D39" si="35">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C39&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;U&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E39" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>323</v>
+      </c>
+      <c r="C40" t="s">
+        <v>224</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" ref="D40" si="36">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C40&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;U2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E40" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>337</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C41" t="s">
+        <v>225</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" ref="D41" si="37">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C41&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;X&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E41" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>339</v>
+      </c>
+      <c r="C42" t="s">
+        <v>226</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" ref="D42" si="38">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C42&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;X2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E42" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="C34" t="s">
-        <v>219</v>
-      </c>
-      <c r="D34">
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>355</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C43" t="s">
+        <v>227</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" ref="D43" si="39">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C43&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;Y&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E43" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>357</v>
+      </c>
+      <c r="C44" t="s">
+        <v>228</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" ref="D44" si="40">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C44&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;Y2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E44" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="1" t="s">
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>371</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C35" t="s">
-        <v>220</v>
-      </c>
-      <c r="D35">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="C36" t="s">
-        <v>221</v>
-      </c>
-      <c r="D36">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="1" t="s">
+      <c r="C45" t="s">
+        <v>229</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" ref="D45" si="41">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C45&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;Z&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E45" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>373</v>
+      </c>
+      <c r="C46" t="s">
+        <v>230</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" ref="D46" si="42">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C46&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;Z2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E46" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>387</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C37" t="s">
-        <v>222</v>
-      </c>
-      <c r="D37">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="C38" t="s">
-        <v>223</v>
-      </c>
-      <c r="D38">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C39" t="s">
-        <v>224</v>
-      </c>
-      <c r="D39">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="C40" t="s">
-        <v>225</v>
-      </c>
-      <c r="D40">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C41" t="s">
-        <v>226</v>
-      </c>
-      <c r="D41">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="C42" t="s">
-        <v>227</v>
-      </c>
-      <c r="D42">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C43" t="s">
-        <v>228</v>
-      </c>
-      <c r="D43">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="C44" t="s">
-        <v>229</v>
-      </c>
-      <c r="D44">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C45" t="s">
-        <v>230</v>
-      </c>
-      <c r="D45">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>231</v>
       </c>
-      <c r="D46">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="D47" t="str">
+        <f t="shared" ref="D47" si="43">"&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;"&amp;C47&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw type=%catch%&gt;&lt;seg rend=%smallcaps%&gt;&lt;choice&gt;&lt;abbr&gt;Vol.&lt;/abbr&gt;&lt;expan&gt;Volume&lt;/expan&gt;&lt;/choice&gt; I.&lt;/seg&gt;&lt;seg rend=%right%&gt;2A&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E47" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>389</v>
+      </c>
+      <c r="C48" t="s">
         <v>232</v>
       </c>
-      <c r="D47">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="C48" t="s">
-        <v>233</v>
-      </c>
-      <c r="D48">
-        <v>389</v>
+      <c r="D48" t="str">
+        <f t="shared" ref="D48" si="44">"&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;"&amp;C48&amp;"&lt;/seg&gt;&lt;/fw&gt;"</f>
+        <v>&lt;fw place=%inspace%&gt;&lt;seg rend=%right%&gt;2A2&lt;/seg&gt;&lt;/fw&gt;</v>
+      </c>
+      <c r="E48" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>